<commit_message>
Improve min value method
</commit_message>
<xml_diff>
--- a/output/range_output/Comparisons-no-sliding-vs-sliding.xlsx
+++ b/output/range_output/Comparisons-no-sliding-vs-sliding.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcchanaka/PycharmProjects/Research-Proj-NetEmb/output/range_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABF7C23-6242-394E-A16A-2C9DDB22B79D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7268817-FF4D-3C45-B76D-27843B79A455}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{E0D25737-D57C-E047-BB88-DD40C276A45C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>1CDX1</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>No sliding window</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>low</t>
   </si>
 </sst>
 </file>
@@ -165,13 +174,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,32 +499,32 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -552,7 +561,7 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -587,7 +596,7 @@
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -622,7 +631,7 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -676,24 +685,24 @@
     </row>
     <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="H12" s="4"/>
+      <c r="J12" s="4"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -718,7 +727,7 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
@@ -741,7 +750,7 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
@@ -764,7 +773,7 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
@@ -786,52 +795,110 @@
       </c>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>977</v>
+      </c>
+      <c r="D20">
+        <v>1652</v>
+      </c>
+      <c r="E20">
+        <v>8045</v>
+      </c>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1327</v>
+      </c>
+      <c r="D21">
+        <v>2580</v>
+      </c>
+      <c r="E21">
+        <v>16810</v>
+      </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>725</v>
+      </c>
+      <c r="D22">
+        <v>1834</v>
+      </c>
+      <c r="E22">
+        <v>6778</v>
+      </c>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>1044</v>
+      </c>
+      <c r="D23">
+        <v>2000</v>
+      </c>
+      <c r="E23">
+        <v>6059</v>
+      </c>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="12:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="12:12" ht="17" x14ac:dyDescent="0.2">
@@ -839,12 +906,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>